<commit_message>
add data to stable upright experiment statistics
</commit_message>
<xml_diff>
--- a/test results/birth to stable upright results.xlsx
+++ b/test results/birth to stable upright results.xlsx
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -537,7 +537,14 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="H8">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>